<commit_message>
stabilize cleaning files & internal validity analysis for number of pawns balance
</commit_message>
<xml_diff>
--- a/Tables/censoring_imp.xlsx
+++ b/Tables/censoring_imp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6BAAB2-6C91-443D-B28C-7BDF53252071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C411AE-97EC-4148-908D-6ABCD7C6C23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16005" yWindow="-9510" windowWidth="14400" windowHeight="8175" xr2:uid="{C3D25F1B-BFB2-4591-A36B-F58AE69A34DA}"/>
+    <workbookView xWindow="-18495" yWindow="-12000" windowWidth="21600" windowHeight="11235" xr2:uid="{C3D25F1B-BFB2-4591-A36B-F58AE69A34DA}"/>
   </bookViews>
   <sheets>
     <sheet name="censoring_imp" sheetId="1" r:id="rId1"/>
@@ -304,19 +304,19 @@
         </row>
         <row r="5">
           <cell r="B5" t="str">
-            <v>-234.6***</v>
+            <v>-236.0***</v>
           </cell>
           <cell r="C5" t="str">
-            <v>-191.8***</v>
+            <v>-191.7***</v>
           </cell>
           <cell r="D5" t="str">
-            <v>0.089</v>
+            <v>-0.63</v>
           </cell>
           <cell r="E5" t="str">
-            <v>-74.5**</v>
+            <v>-75.9**</v>
           </cell>
           <cell r="F5" t="str">
-            <v>-0.063***</v>
+            <v>-0.064***</v>
           </cell>
           <cell r="G5" t="str">
             <v>-0.14***</v>
@@ -333,7 +333,7 @@
             <v>(37.6)</v>
           </cell>
           <cell r="D6" t="str">
-            <v>(2.77)</v>
+            <v>(3.01)</v>
           </cell>
           <cell r="E6" t="str">
             <v>(30.5)</v>
@@ -385,7 +385,7 @@
             <v>0.019</v>
           </cell>
           <cell r="G9" t="str">
-            <v>0.042</v>
+            <v>0.043</v>
           </cell>
         </row>
         <row r="10">
@@ -393,19 +393,19 @@
             <v>Control Mean</v>
           </cell>
           <cell r="B10" t="str">
-            <v>988.6</v>
+            <v>989.9</v>
           </cell>
           <cell r="C10" t="str">
             <v>593.4</v>
           </cell>
           <cell r="D10" t="str">
-            <v>5.26</v>
+            <v>5.96</v>
           </cell>
           <cell r="E10" t="str">
-            <v>395.2</v>
+            <v>396.5</v>
           </cell>
           <cell r="F10" t="str">
-            <v>0.43</v>
+            <v>0.44</v>
           </cell>
           <cell r="G10" t="str">
             <v>0.61</v>
@@ -435,22 +435,22 @@
         </row>
         <row r="5">
           <cell r="B5" t="str">
-            <v>-189.9***</v>
+            <v>-191.2***</v>
           </cell>
           <cell r="C5" t="str">
             <v>-207.7***</v>
           </cell>
           <cell r="D5" t="str">
-            <v>1.89</v>
+            <v>1.17</v>
           </cell>
           <cell r="E5" t="str">
-            <v>-13.8</v>
+            <v>-15.1</v>
           </cell>
           <cell r="F5" t="str">
-            <v>0.0094</v>
+            <v>0.0083</v>
           </cell>
           <cell r="G5" t="str">
-            <v>-0.073***</v>
+            <v>-0.076***</v>
           </cell>
         </row>
         <row r="6">
@@ -464,7 +464,7 @@
             <v>(37.4)</v>
           </cell>
           <cell r="D6" t="str">
-            <v>(3.24)</v>
+            <v>(3.45)</v>
           </cell>
           <cell r="E6" t="str">
             <v>(31.2)</v>
@@ -507,7 +507,7 @@
             <v>0.026</v>
           </cell>
           <cell r="D9" t="str">
-            <v>0.003</v>
+            <v>0.004</v>
           </cell>
           <cell r="E9" t="str">
             <v>0.009</v>
@@ -516,7 +516,7 @@
             <v>0.014</v>
           </cell>
           <cell r="G9" t="str">
-            <v>0.022</v>
+            <v>0.023</v>
           </cell>
         </row>
         <row r="10">
@@ -524,19 +524,19 @@
             <v>Control Mean</v>
           </cell>
           <cell r="B10" t="str">
-            <v>988.6</v>
+            <v>989.9</v>
           </cell>
           <cell r="C10" t="str">
             <v>593.4</v>
           </cell>
           <cell r="D10" t="str">
-            <v>5.26</v>
+            <v>5.96</v>
           </cell>
           <cell r="E10" t="str">
-            <v>395.2</v>
+            <v>396.5</v>
           </cell>
           <cell r="F10" t="str">
-            <v>0.43</v>
+            <v>0.44</v>
           </cell>
           <cell r="G10" t="str">
             <v>0.61</v>
@@ -823,82 +823,82 @@
       <sheetData sheetId="0">
         <row r="5">
           <cell r="B5" t="str">
-            <v>-262.6***</v>
+            <v>-264.9***</v>
           </cell>
           <cell r="C5" t="str">
-            <v>-170.7***</v>
+            <v>-169.6***</v>
           </cell>
           <cell r="D5" t="str">
-            <v>-0.56</v>
+            <v>-1.43</v>
           </cell>
           <cell r="E5" t="str">
-            <v>-123.9***</v>
+            <v>-127.4***</v>
           </cell>
           <cell r="F5" t="str">
             <v>-0.12***</v>
           </cell>
           <cell r="G5" t="str">
-            <v>-0.16***</v>
+            <v>-0.17***</v>
           </cell>
         </row>
         <row r="6">
           <cell r="B6" t="str">
-            <v>(53.3)</v>
+            <v>(53.8)</v>
           </cell>
           <cell r="C6" t="str">
-            <v>(37.3)</v>
+            <v>(37.2)</v>
           </cell>
           <cell r="D6" t="str">
-            <v>(3.30)</v>
+            <v>(3.52)</v>
           </cell>
           <cell r="E6" t="str">
-            <v>(32.5)</v>
+            <v>(33.1)</v>
           </cell>
           <cell r="F6" t="str">
-            <v>(0.024)</v>
+            <v>(0.025)</v>
           </cell>
           <cell r="G6" t="str">
-            <v>(0.027)</v>
+            <v>(0.028)</v>
           </cell>
         </row>
         <row r="8">
           <cell r="B8" t="str">
-            <v>-39.5</v>
+            <v>-42.4</v>
           </cell>
           <cell r="C8" t="str">
-            <v>-30.5</v>
+            <v>-29.1</v>
           </cell>
           <cell r="D8" t="str">
-            <v>-2.71</v>
+            <v>-2.66</v>
           </cell>
           <cell r="E8" t="str">
-            <v>-10.4</v>
+            <v>-14.6</v>
           </cell>
           <cell r="F8" t="str">
-            <v>-0.014</v>
+            <v>-0.017</v>
           </cell>
           <cell r="G8" t="str">
-            <v>0.0060</v>
+            <v>0.0026</v>
           </cell>
         </row>
         <row r="9">
           <cell r="B9" t="str">
-            <v>(56.4)</v>
+            <v>(56.9)</v>
           </cell>
           <cell r="C9" t="str">
-            <v>(41.9)</v>
+            <v>(41.8)</v>
           </cell>
           <cell r="D9" t="str">
-            <v>(2.75)</v>
+            <v>(3.24)</v>
           </cell>
           <cell r="E9" t="str">
-            <v>(34.4)</v>
+            <v>(34.9)</v>
           </cell>
           <cell r="F9" t="str">
             <v>(0.024)</v>
           </cell>
           <cell r="G9" t="str">
-            <v>(0.028)</v>
+            <v>(0.029)</v>
           </cell>
         </row>
         <row r="11">
@@ -923,16 +923,16 @@
         </row>
         <row r="12">
           <cell r="B12" t="str">
-            <v>0.017</v>
+            <v>0.018</v>
           </cell>
           <cell r="C12" t="str">
             <v>0.022</v>
           </cell>
           <cell r="D12" t="str">
-            <v>0.003</v>
+            <v>0.002</v>
           </cell>
           <cell r="E12" t="str">
-            <v>0.009</v>
+            <v>0.010</v>
           </cell>
           <cell r="F12" t="str">
             <v>0.016</v>
@@ -943,19 +943,19 @@
         </row>
         <row r="13">
           <cell r="B13" t="str">
-            <v>1029.8</v>
+            <v>1034.5</v>
           </cell>
           <cell r="C13" t="str">
-            <v>565.8</v>
+            <v>563.4</v>
           </cell>
           <cell r="D13" t="str">
-            <v>7.06</v>
+            <v>7.69</v>
           </cell>
           <cell r="E13" t="str">
-            <v>463.9</v>
+            <v>471.2</v>
           </cell>
           <cell r="F13" t="str">
-            <v>0.51</v>
+            <v>0.52</v>
           </cell>
           <cell r="G13" t="str">
             <v>0.66</v>
@@ -1350,23 +1350,23 @@
       </c>
       <c r="B5" s="2" t="str">
         <f>[1]decomposition_main_te_0_0!B5</f>
-        <v>-234.6***</v>
+        <v>-236.0***</v>
       </c>
       <c r="C5" s="2" t="str">
         <f>[1]decomposition_main_te_0_0!C5</f>
-        <v>-191.8***</v>
+        <v>-191.7***</v>
       </c>
       <c r="D5" s="2" t="str">
         <f>[1]decomposition_main_te_0_0!D5</f>
-        <v>0.089</v>
+        <v>-0.63</v>
       </c>
       <c r="E5" s="2" t="str">
         <f>[1]decomposition_main_te_0_0!E5</f>
-        <v>-74.5**</v>
+        <v>-75.9**</v>
       </c>
       <c r="F5" s="2" t="str">
         <f>[1]decomposition_main_te_0_0!F5</f>
-        <v>-0.063***</v>
+        <v>-0.064***</v>
       </c>
       <c r="G5" s="2" t="str">
         <f>[1]decomposition_main_te_0_0!G5</f>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="D6" s="2" t="str">
         <f>[1]decomposition_main_te_0_0!D6</f>
-        <v>(2.77)</v>
+        <v>(3.01)</v>
       </c>
       <c r="E6" s="2" t="str">
         <f>[1]decomposition_main_te_0_0!E6</f>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="G9" s="2" t="str">
         <f>[1]decomposition_main_te_0_0!G9</f>
-        <v>0.042</v>
+        <v>0.043</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="B10" s="5" t="str">
         <f>[1]decomposition_main_te_0_0!B10</f>
-        <v>988.6</v>
+        <v>989.9</v>
       </c>
       <c r="C10" s="5" t="str">
         <f>[1]decomposition_main_te_0_0!C10</f>
@@ -1477,15 +1477,15 @@
       </c>
       <c r="D10" s="5" t="str">
         <f>[1]decomposition_main_te_0_0!D10</f>
-        <v>5.26</v>
+        <v>5.96</v>
       </c>
       <c r="E10" s="5" t="str">
         <f>[1]decomposition_main_te_0_0!E10</f>
-        <v>395.2</v>
+        <v>396.5</v>
       </c>
       <c r="F10" s="5" t="str">
         <f>[1]decomposition_main_te_0_0!F10</f>
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="G10" s="5" t="str">
         <f>[1]decomposition_main_te_0_0!G10</f>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B14" s="2" t="str">
         <f>[2]decomposition_main_te_0_1!B5</f>
-        <v>-189.9***</v>
+        <v>-191.2***</v>
       </c>
       <c r="C14" s="2" t="str">
         <f>[2]decomposition_main_te_0_1!C5</f>
@@ -1553,19 +1553,19 @@
       </c>
       <c r="D14" s="2" t="str">
         <f>[2]decomposition_main_te_0_1!D5</f>
-        <v>1.89</v>
+        <v>1.17</v>
       </c>
       <c r="E14" s="2" t="str">
         <f>[2]decomposition_main_te_0_1!E5</f>
-        <v>-13.8</v>
+        <v>-15.1</v>
       </c>
       <c r="F14" s="2" t="str">
         <f>[2]decomposition_main_te_0_1!F5</f>
-        <v>0.0094</v>
+        <v>0.0083</v>
       </c>
       <c r="G14" s="2" t="str">
         <f>[2]decomposition_main_te_0_1!G5</f>
-        <v>-0.073***</v>
+        <v>-0.076***</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="D15" s="2" t="str">
         <f>[2]decomposition_main_te_0_1!D6</f>
-        <v>(3.24)</v>
+        <v>(3.45)</v>
       </c>
       <c r="E15" s="2" t="str">
         <f>[2]decomposition_main_te_0_1!E6</f>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="D18" s="2" t="str">
         <f>[2]decomposition_main_te_0_1!D9</f>
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="E18" s="2" t="str">
         <f>[2]decomposition_main_te_0_1!E9</f>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="G18" s="2" t="str">
         <f>[2]decomposition_main_te_0_1!G9</f>
-        <v>0.022</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="B19" s="5" t="str">
         <f>[2]decomposition_main_te_0_1!B10</f>
-        <v>988.6</v>
+        <v>989.9</v>
       </c>
       <c r="C19" s="5" t="str">
         <f>[2]decomposition_main_te_0_1!C10</f>
@@ -1672,15 +1672,15 @@
       </c>
       <c r="D19" s="5" t="str">
         <f>[2]decomposition_main_te_0_1!D10</f>
-        <v>5.26</v>
+        <v>5.96</v>
       </c>
       <c r="E19" s="5" t="str">
         <f>[2]decomposition_main_te_0_1!E10</f>
-        <v>395.2</v>
+        <v>396.5</v>
       </c>
       <c r="F19" s="5" t="str">
         <f>[2]decomposition_main_te_0_1!F10</f>
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="G19" s="5" t="str">
         <f>[2]decomposition_main_te_0_1!G10</f>
@@ -2096,19 +2096,19 @@
       </c>
       <c r="B41" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!B5</f>
-        <v>-262.6***</v>
+        <v>-264.9***</v>
       </c>
       <c r="C41" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!C5</f>
-        <v>-170.7***</v>
+        <v>-169.6***</v>
       </c>
       <c r="D41" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!D5</f>
-        <v>-0.56</v>
+        <v>-1.43</v>
       </c>
       <c r="E41" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!E5</f>
-        <v>-123.9***</v>
+        <v>-127.4***</v>
       </c>
       <c r="F41" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!F5</f>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="G41" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!G5</f>
-        <v>-0.16***</v>
+        <v>-0.17***</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -2125,27 +2125,27 @@
       </c>
       <c r="B42" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!B6</f>
-        <v>(53.3)</v>
+        <v>(53.8)</v>
       </c>
       <c r="C42" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!C6</f>
-        <v>(37.3)</v>
+        <v>(37.2)</v>
       </c>
       <c r="D42" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!D6</f>
-        <v>(3.30)</v>
+        <v>(3.52)</v>
       </c>
       <c r="E42" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!E6</f>
-        <v>(32.5)</v>
+        <v>(33.1)</v>
       </c>
       <c r="F42" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!F6</f>
-        <v>(0.024)</v>
+        <v>(0.025)</v>
       </c>
       <c r="G42" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!G6</f>
-        <v>(0.027)</v>
+        <v>(0.028)</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -2154,45 +2154,45 @@
       </c>
       <c r="B43" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!B8</f>
-        <v>-39.5</v>
+        <v>-42.4</v>
       </c>
       <c r="C43" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!C8</f>
-        <v>-30.5</v>
+        <v>-29.1</v>
       </c>
       <c r="D43" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!D8</f>
-        <v>-2.71</v>
+        <v>-2.66</v>
       </c>
       <c r="E43" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!E8</f>
-        <v>-10.4</v>
+        <v>-14.6</v>
       </c>
       <c r="F43" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!F8</f>
-        <v>-0.014</v>
+        <v>-0.017</v>
       </c>
       <c r="G43" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!G8</f>
-        <v>0.0060</v>
+        <v>0.0026</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!B9</f>
-        <v>(56.4)</v>
+        <v>(56.9)</v>
       </c>
       <c r="C44" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!C9</f>
-        <v>(41.9)</v>
+        <v>(41.8)</v>
       </c>
       <c r="D44" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!D9</f>
-        <v>(2.75)</v>
+        <v>(3.24)</v>
       </c>
       <c r="E44" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!E9</f>
-        <v>(34.4)</v>
+        <v>(34.9)</v>
       </c>
       <c r="F44" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!F9</f>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="G44" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!G9</f>
-        <v>(0.028)</v>
+        <v>(0.029)</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="B47" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!B12</f>
-        <v>0.017</v>
+        <v>0.018</v>
       </c>
       <c r="C47" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!C12</f>
@@ -2246,11 +2246,11 @@
       </c>
       <c r="D47" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!D12</f>
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="E47" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!E12</f>
-        <v>0.009</v>
+        <v>0.010</v>
       </c>
       <c r="F47" s="2" t="str">
         <f>[5]decomposition_main_te_imppr!F12</f>
@@ -2267,23 +2267,23 @@
       </c>
       <c r="B48" s="5" t="str">
         <f>[5]decomposition_main_te_imppr!B13</f>
-        <v>1029.8</v>
+        <v>1034.5</v>
       </c>
       <c r="C48" s="5" t="str">
         <f>[5]decomposition_main_te_imppr!C13</f>
-        <v>565.8</v>
+        <v>563.4</v>
       </c>
       <c r="D48" s="5" t="str">
         <f>[5]decomposition_main_te_imppr!D13</f>
-        <v>7.06</v>
+        <v>7.69</v>
       </c>
       <c r="E48" s="5" t="str">
         <f>[5]decomposition_main_te_imppr!E13</f>
-        <v>463.9</v>
+        <v>471.2</v>
       </c>
       <c r="F48" s="5" t="str">
         <f>[5]decomposition_main_te_imppr!F13</f>
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="G48" s="5" t="str">
         <f>[5]decomposition_main_te_imppr!G13</f>

</xml_diff>